<commit_message>
chaned format of 'date' columns
</commit_message>
<xml_diff>
--- a/Naver/Results/FD_Crawling_Naver_Blog_Archaive/FD_Crawling_Naver_Blog_20240829.xlsx
+++ b/Naver/Results/FD_Crawling_Naver_Blog_Archaive/FD_Crawling_Naver_Blog_20240829.xlsx
@@ -481,39 +481,37 @@
           <t>Naver Blog</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>20240829</t>
-        </is>
+      <c r="B2" t="n">
+        <v>20240829</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>강남N타워 맛집 역삼 파스타바 파브란트</t>
+          <t>강남역고기집 우대포 먹방 유튜버도 반한 소갈비 맛집</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://blog.naver.com/winendine2017/223564698837</t>
+          <t>https://blog.naver.com/suzy_blog/223564812454</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>파브란트</t>
+          <t>우대포 강남역점</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>서울특별시 강남구 테헤란로 129 지하2층 B246호</t>
+          <t>서울특별시 강남구 강남대로94길 11 1층</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>#강남n타워맛집, #강남역파스타, #강남역소개팅, #역삼파스타, #역삼맛집, #파브란트, #강남역데이트, #역삼역데이트, #강남데이트, #강남맛집, #강남파스타, #역삼역파스타, #파스타바, #역삼파스타바, #강남역파스타바</t>
+          <t>#역삼문화공원제1호공영주차장, #우대포, #강남역맛집, #강남역고기집, #역삼동맛집, #강남역회식, #강남역소고기, #강남역고기, #강남역모임, #강남역저녁, #강남역11번출구맛집</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2024-08-29 11:30</t>
+          <t>2024-08-29 12:52</t>
         </is>
       </c>
     </row>
@@ -523,39 +521,37 @@
           <t>Naver Blog</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>20240829</t>
-        </is>
+      <c r="B3" t="n">
+        <v>20240829</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>영덕 강구항 대게 맛집 영덕대게궁 가격</t>
+          <t>오산 고기 맛집 소오산 오산대역 최고의 소고기 B세트 후기</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://blog.naver.com/ggoulggoul/223564649477</t>
+          <t>https://blog.naver.com/omytheo/223564807189</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>영덕대게궁</t>
+          <t>소오산</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>경상북도 영덕군 강구면 강구대게길 29 영덕대게궁</t>
+          <t>경기도 오산시 내삼미로79번길 26 107, 108호</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>#영덕대게맛집, #영덕강구항대게맛집, #강구항대게맛집, #강구항맛집, #영덕대게가격, #영덕대게궁가격, #영덕대게궁, #영덕강구항맛집, #영덕대게, #영덕가볼만한곳, #영덕대게거리, #대게코스요리, #영덕대게거리맛집, #대게宮, #대게궁</t>
+          <t>#소오산, #오산고기맛집, #오산대역맛집, #소갈비살, #오산소갈비살, #오산모임, #오산회식, #가성비회식장소, #숯불소고기</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2024-08-29 11:30</t>
+          <t>2024-08-29 12:52</t>
         </is>
       </c>
     </row>
@@ -565,39 +561,37 @@
           <t>Naver Blog</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>20240829</t>
-        </is>
+      <c r="B4" t="n">
+        <v>20240829</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>강남역 횟집 속초오징어어시장 가성비 횟집 추천 내돈내산</t>
+          <t>강남N타워 맛집 역삼 파스타바 파브란트</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://blog.naver.com/qnwkqortnn/223564770076</t>
+          <t>https://blog.naver.com/winendine2017/223564698837</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>속초오징어어시장 강남역점</t>
+          <t>파브란트</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>서울특별시 강남구 강남대로78길 16 1층</t>
+          <t>서울특별시 강남구 테헤란로 129 지하2층 B246호</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>#강남역횟집, #강남역가성비횟집, #속초오징어어시장강남역, #강남회식장소추천</t>
+          <t>#강남n타워맛집, #강남역파스타, #강남역소개팅, #역삼파스타, #역삼맛집, #파브란트, #강남역데이트, #역삼역데이트, #강남데이트, #강남맛집, #강남파스타, #역삼역파스타, #파스타바, #역삼파스타바, #강남역파스타바</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2024-08-29 11:30</t>
+          <t>2024-08-29 12:52</t>
         </is>
       </c>
     </row>
@@ -607,39 +601,37 @@
           <t>Naver Blog</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>20240829</t>
-        </is>
+      <c r="B5" t="n">
+        <v>20240829</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>원주 무실동 맛집 추천 점심 물회 부산횟집</t>
+          <t>영덕 강구항 대게 맛집 영덕대게궁 가격</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://blog.naver.com/s2ll27/223564642896</t>
+          <t>https://blog.naver.com/ggoulggoul/223564649477</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>부산횟집</t>
+          <t>영덕대게궁</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>강원특별자치도 원주시 만대공원길 56</t>
+          <t>경상북도 영덕군 강구면 강구대게길 29 영덕대게궁</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>#원주무실동맛집, #원주점심맛집, #원주물회맛집, #원주부산횟집, #원주맛집추천, #원주무실동맛집추천</t>
+          <t>#영덕대게맛집, #영덕강구항대게맛집, #강구항대게맛집, #강구항맛집, #영덕대게가격, #영덕대게궁가격, #영덕대게궁, #영덕강구항맛집, #영덕대게, #영덕가볼만한곳, #영덕대게거리, #대게코스요리, #영덕대게거리맛집, #대게宮, #대게궁</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2024-08-29 11:30</t>
+          <t>2024-08-29 12:52</t>
         </is>
       </c>
     </row>
@@ -649,39 +641,37 @@
           <t>Naver Blog</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>20240829</t>
-        </is>
+      <c r="B6" t="n">
+        <v>20240829</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>숙대입구역 맛집 마구로참치 특수부위까지 즐기는 지중해 생참치</t>
+          <t>동래 맛집 야키니쿠가 맛있는 현지 감성의 모토이시 공격 후기</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://blog.naver.com/enviableb/223564632129</t>
+          <t>https://blog.naver.com/ganzzajang/223562794470</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>마구로참치</t>
+          <t>모토이시 동래점</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>서울특별시 용산구 한강대로 271</t>
+          <t>부산광역시 동래구 충렬대로181번길 65 1~2층</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>#숙대입구역맛집, #마구로참치, #숙대입구맛집, #남영역맛집, #갈월동맛집, #용산참치, #남영동맛집, #숙대입구횟집, #남영역횟집, #용산횟집, #용산룸식당, #서울참치맛집</t>
+          <t>#동래맛집, #동래역맛집, #동래술집, #동래술집추천, #동래고기집, #동래역술집, #명륜동맛집, #동래역고깃집, #부산야끼니꾸, #동래야끼니꾸, #동래와규</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2024-08-29 11:30</t>
+          <t>2024-08-29 12:52</t>
         </is>
       </c>
     </row>
@@ -691,39 +681,37 @@
           <t>Naver Blog</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>20240829</t>
-        </is>
+      <c r="B7" t="n">
+        <v>20240829</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>강남역고기집 우대포 먹방 유튜버도 반한 소갈비 맛집</t>
+          <t>수원 행궁동 한옥 카페 카페도화 연무대점 행리단길 디저트 맛집</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://blog.naver.com/suzy_blog/223564812454</t>
+          <t>https://blog.naver.com/greenmoom46/223564828431</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>우대포 강남역점</t>
+          <t>카페도화 연무대점</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>서울특별시 강남구 강남대로94길 11 1층</t>
+          <t>경기도 수원시 팔달구 창룡대로103번길 8 2층</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>#역삼문화공원제1호공영주차장, #우대포, #강남역맛집, #강남역고기집, #역삼동맛집, #강남역회식, #강남역소고기, #강남역고기, #강남역모임, #강남역저녁, #강남역11번출구맛집</t>
+          <t>#행궁동브런치, #수원브런치, #행궁동와인바, #수원한옥카페, #행궁동한옥카페, #맛띠유, #맛집탐구기</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2024-08-29 11:30</t>
+          <t>2024-08-29 12:52</t>
         </is>
       </c>
     </row>
@@ -733,39 +721,37 @@
           <t>Naver Blog</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>20240829</t>
-        </is>
+      <c r="B8" t="n">
+        <v>20240829</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>오산 고기 맛집 소오산 오산대역 최고의 소고기 B세트 후기</t>
+          <t>석촌역 맛집, 청결하고 맛있는 숯불구이 '2층 통돼지집' 후기</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://blog.naver.com/omytheo/223564807189</t>
+          <t>https://blog.naver.com/gintonicdays/223564775499</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>소오산</t>
+          <t>2층 통돼지집</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>경기도 오산시 내삼미로79번길 26 107, 108호</t>
+          <t>서울특별시 송파구 백제고분로 384 2층 201호(송파동, 평화빌딩)</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>#소오산, #오산고기맛집, #오산대역맛집, #소갈비살, #오산소갈비살, #오산모임, #오산회식, #가성비회식장소, #숯불소고기</t>
+          <t>#2층통돼지집, #잠실맛집, #송파맛집, #석촌역맛집, #돼지두루치기, #돼지숯불구이, #갈비살구이, #테진아제조, #벌집껍데기, #잠실회식장소, #잠실모임장소, #잠실고기맛집, #석촌역고기맛집, #송파동고기집, #송파동고기맛집, #송파동맛집, #롯데타워뷰</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2024-08-29 11:30</t>
+          <t>2024-08-29 12:52</t>
         </is>
       </c>
     </row>
@@ -775,39 +761,37 @@
           <t>Naver Blog</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>20240829</t>
-        </is>
+      <c r="B9" t="n">
+        <v>20240829</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>두툼한 통삼겹이 통째로 김치찌개 의정부맛집 오남매솥밥</t>
+          <t>강남역 횟집 속초오징어어시장 가성비 횟집 추천 내돈내산</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://blog.naver.com/hahadanro/223562750525</t>
+          <t>https://blog.naver.com/qnwkqortnn/223564770076</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>오남매솥밥</t>
+          <t>속초오징어어시장 강남역점</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>경기도 의정부시 오목로225번길 23-3 1층 오남매클라스</t>
+          <t>서울특별시 강남구 강남대로78길 16 1층</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>#오남매솥밥, #민락동맛집, #한식맛집, #의정부맛집, #의정부김치찌개, #김치찌개, #통삽겹김치찜</t>
+          <t>#강남역횟집, #강남역가성비횟집, #속초오징어어시장강남역, #강남회식장소추천</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2024-08-29 11:30</t>
+          <t>2024-08-29 12:52</t>
         </is>
       </c>
     </row>
@@ -817,39 +801,37 @@
           <t>Naver Blog</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>20240829</t>
-        </is>
+      <c r="B10" t="n">
+        <v>20240829</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>왕림휴게소 근처 동천홍 봉담점 마라 짬뽕 맛집</t>
+          <t>원주 무실동 맛집 추천 점심 물회 부산횟집</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://blog.naver.com/ddomuz/223564273757</t>
+          <t>https://blog.naver.com/s2ll27/223564642896</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>동천홍 봉담점</t>
+          <t>부산횟집</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>경기도 화성시 봉담읍 삼천병마로 1079-12</t>
+          <t>강원특별자치도 원주시 만대공원길 56</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>#동천홍, #동천홍봉담점, #왕림휴게소맛집, #봉담중국집, #봉담짬뽕맛집, #봉담마라짬뽕, #봉담짜장면, #봉담중식당, #봉담가족모임</t>
+          <t>#원주무실동맛집, #원주점심맛집, #원주물회맛집, #원주부산횟집, #원주맛집추천, #원주무실동맛집추천</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2024-08-29 11:30</t>
+          <t>2024-08-29 12:52</t>
         </is>
       </c>
     </row>
@@ -859,39 +841,37 @@
           <t>Naver Blog</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>20240829</t>
-        </is>
+      <c r="B11" t="n">
+        <v>20240829</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>양재역 맛집 미면정 양재본점 만두칼국수 가족모임 추천</t>
+          <t>숙대입구역 맛집 마구로참치 특수부위까지 즐기는 지중해 생참치</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://blog.naver.com/ykheeee9500/223564513957</t>
+          <t>https://blog.naver.com/enviableb/223564632129</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>미면정 양재본점</t>
+          <t>마구로참치</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>서울특별시 강남구 남부순환로365길 22 오이빌딩 2층</t>
+          <t>서울특별시 용산구 한강대로 271</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>#양재역맛집, #양재역맛집미면정, #미면정양재본점, #만두칼국수맛집, #한국음식장인이만드는미면정</t>
+          <t>#숙대입구역맛집, #마구로참치, #숙대입구맛집, #남영역맛집, #갈월동맛집, #용산참치, #남영동맛집, #숙대입구횟집, #남영역횟집, #용산횟집, #용산룸식당, #서울참치맛집</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2024-08-29 11:30</t>
+          <t>2024-08-29 12:52</t>
         </is>
       </c>
     </row>
@@ -901,39 +881,37 @@
           <t>Naver Blog</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>20240829</t>
-        </is>
+      <c r="B12" t="n">
+        <v>20240829</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>강남구청역 카페 트롬바커피 에그타르트맛집</t>
+          <t>두툼한 통삼겹이 통째로 김치찌개 의정부맛집 오남매솥밥</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://blog.naver.com/kcy2736/223564554138</t>
+          <t>https://blog.naver.com/hahadanro/223562750525</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>트롬바커피</t>
+          <t>오남매솥밥</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>서울특별시 강남구 선릉로126길 12 1층</t>
+          <t>경기도 의정부시 오목로225번길 23-3 1층 오남매클라스</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>#서이추환영, #삼성동카페, #강남구청대저트카페, #삼성동디저트카페</t>
+          <t>#오남매솥밥, #민락동맛집, #한식맛집, #의정부맛집, #의정부김치찌개, #김치찌개, #통삽겹김치찜</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2024-08-29 11:30</t>
+          <t>2024-08-29 12:52</t>
         </is>
       </c>
     </row>
@@ -943,31 +921,37 @@
           <t>Naver Blog</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>20240828</t>
-        </is>
+      <c r="B13" t="n">
+        <v>20240829</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>다양한 토핑의 매력 요아정 꿀조합 벌꿀 요거트아이스크림 오창점 배달</t>
+          <t>왕림휴게소 근처 동천홍 봉담점 마라 짬뽕 맛집</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://blog.naver.com/maboo37/223564409145</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
+          <t>https://blog.naver.com/ddomuz/223564273757</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>동천홍 봉담점</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>경기도 화성시 봉담읍 삼천병마로 1079-12</t>
+        </is>
+      </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>#협찬, #요거트아이스크림의정석, #요거트아이스크림, #생과일아이스크림, #요거트, #그릭요거트, #그릭요거트전문점, #요거트아이스크림전문점, #카페프랜차이즈, #요거트프랜차이즈, #yogurt, #greek, #디저트, #디저트맛집, #자사앱, #앱, #요아정앱, #할인쿠폰</t>
+          <t>#동천홍, #동천홍봉담점, #왕림휴게소맛집, #봉담중국집, #봉담짬뽕맛집, #봉담마라짬뽕, #봉담짜장면, #봉담중식당, #봉담가족모임</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2024-08-29 11:30</t>
+          <t>2024-08-29 12:52</t>
         </is>
       </c>
     </row>
@@ -977,39 +961,37 @@
           <t>Naver Blog</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>20240829</t>
-        </is>
+      <c r="B14" t="n">
+        <v>20240829</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>원주시청 근처 근사한 원주 한우 맛집 고기삼촌 후기</t>
+          <t>양재역 맛집 미면정 양재본점 만두칼국수 가족모임 추천</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://blog.naver.com/1115hq/223564798254</t>
+          <t>https://blog.naver.com/ykheeee9500/223564513957</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>고기삼촌</t>
+          <t>미면정 양재본점</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>강원특별자치도 원주시 시청로 24 105,106호</t>
+          <t>서울특별시 강남구 남부순환로365길 22 오이빌딩 2층</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>#원주한우맛집, #원주시청맛집</t>
+          <t>#양재역맛집, #양재역맛집미면정, #미면정양재본점, #만두칼국수맛집, #한국음식장인이만드는미면정</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2024-08-29 11:30</t>
+          <t>2024-08-29 12:52</t>
         </is>
       </c>
     </row>
@@ -1019,39 +1001,37 @@
           <t>Naver Blog</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>20240829</t>
-        </is>
+      <c r="B15" t="n">
+        <v>20240829</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>한드케이크_노원 주문제작 예쁜 레터링 케이크 디자인도안 추천</t>
+          <t>강남구청역 카페 트롬바커피 에그타르트맛집</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://blog.naver.com/sophie242/223561781307</t>
+          <t>https://blog.naver.com/kcy2736/223564554138</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>한드케이크</t>
+          <t>트롬바커피</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>서울특별시 노원구 공릉로58다길 5 B1층 한드케이크</t>
+          <t>서울특별시 강남구 선릉로126길 12 1층</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>#노원주문제작케이크, #노원레터링케이크, #하계역케이크, #도시락케이크, #한드케이크, #레터링케이크디자인, #주문제작케이크, #주문제작케이크도안</t>
+          <t>#서이추환영, #삼성동카페, #강남구청대저트카페, #삼성동디저트카페</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2024-08-29 11:30</t>
+          <t>2024-08-29 12:52</t>
         </is>
       </c>
     </row>
@@ -1061,39 +1041,37 @@
           <t>Naver Blog</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>20240829</t>
-        </is>
+      <c r="B16" t="n">
+        <v>20240829</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>부천 캠핑식당 이색적인 옥상휴게소</t>
+          <t>원주시청 근처 근사한 원주 한우 맛집 고기삼촌 후기</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://blog.naver.com/buzafama/223561930435</t>
+          <t>https://blog.naver.com/1115hq/223564798254</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>옥상휴게소</t>
+          <t>고기삼촌</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>경기도 부천시 원미구 부천로 148 1층 전체</t>
+          <t>강원특별자치도 원주시 시청로 24 105,106호</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>#부천캠핑식당, #부천바베큐맛집, #부천캠핑바베큐, #부천캠핑바베큐식당</t>
+          <t>#원주한우맛집, #원주시청맛집</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2024-08-29 11:30</t>
+          <t>2024-08-29 12:52</t>
         </is>
       </c>
     </row>
@@ -1103,39 +1081,37 @@
           <t>Naver Blog</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>20240829</t>
-        </is>
+      <c r="B17" t="n">
+        <v>20240829</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>대구 수성구 술집 고퀄리티 안주에 분위기 좋은 범어동 맛집 한주</t>
+          <t>한드케이크_노원 주문제작 예쁜 레터링 케이크 디자인도안 추천</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://blog.naver.com/ejr8806/223564731432</t>
+          <t>https://blog.naver.com/sophie242/223561781307</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>한주</t>
+          <t>한드케이크</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>대구광역시 수성구 달구벌대로512길 10 1층 한주</t>
+          <t>서울특별시 노원구 공릉로58다길 5 B1층 한드케이크</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>#대구수성구술집, #수성구술집, #한주, #범어동한주, #범어동맛집</t>
+          <t>#노원주문제작케이크, #노원레터링케이크, #하계역케이크, #도시락케이크, #한드케이크, #레터링케이크디자인, #주문제작케이크, #주문제작케이크도안</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2024-08-29 11:30</t>
+          <t>2024-08-29 12:52</t>
         </is>
       </c>
     </row>
@@ -1145,39 +1121,37 @@
           <t>Naver Blog</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>20240829</t>
-        </is>
+      <c r="B18" t="n">
+        <v>20240829</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>판교 술집 하이네켄 생맥주 맛집 챠오바라이트</t>
+          <t>부천 캠핑식당 이색적인 옥상휴게소</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://blog.naver.com/darkyoon85/223564335342</t>
+          <t>https://blog.naver.com/buzafama/223561930435</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>챠오바라이트 판교점</t>
+          <t>옥상휴게소</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>경기도 성남시 분당구 대왕판교로 660 유스페이스1 1층 125호 챠오바라이트</t>
+          <t>경기도 부천시 원미구 부천로 148 1층 전체</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>#판교맛집, #판교술집, #하이네켄, #하이네켄생맥주, #하이네켄생맥주맛집, #챠오바라이트, #생맥주, #첫모금, #맛집추천, #광고</t>
+          <t>#부천캠핑식당, #부천바베큐맛집, #부천캠핑바베큐, #부천캠핑바베큐식당</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2024-08-29 11:30</t>
+          <t>2024-08-29 12:52</t>
         </is>
       </c>
     </row>
@@ -1187,39 +1161,37 @@
           <t>Naver Blog</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>20240829</t>
-        </is>
+      <c r="B19" t="n">
+        <v>20240829</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>연남동 국숯집 남발카세 팝업 - 젊고 내공 뛰어난 남발게 김준승 셰프님의 새롭고 기발하고 훌륭한 해산물 요리 잔치</t>
+          <t>대구 수성구 술집 고퀄리티 안주에 분위기 좋은 범어동 맛집 한주</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>https://blog.naver.com/zephyr122059/223559250507</t>
+          <t>https://blog.naver.com/ejr8806/223564731432</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>국숯집 연남점</t>
+          <t>한주</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>서울특별시 마포구 동교로34길 21 우측 지층</t>
+          <t>대구광역시 수성구 달구벌대로512길 10 1층 한주</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>#남발게님, #국숯집, #연남동국숯집, #남발카세, #해산물잔치, #국숯집팝업, #남발게님팝업, #연남동남발카세팝업</t>
+          <t>#대구수성구술집, #수성구술집, #한주, #범어동한주, #범어동맛집</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2024-08-29 11:30</t>
+          <t>2024-08-29 12:52</t>
         </is>
       </c>
     </row>
@@ -1229,39 +1201,37 @@
           <t>Naver Blog</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>20240829</t>
-        </is>
+      <c r="B20" t="n">
+        <v>20240829</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>전주 한옥마을 한정식 맛집 - 녹두꽃 건강한 한상차림 #1</t>
+          <t>판교 술집 하이네켄 생맥주 맛집 챠오바라이트</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>https://blog.naver.com/chuchus1216/223564623754</t>
+          <t>https://blog.naver.com/darkyoon85/223564335342</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>녹두꽃</t>
+          <t>챠오바라이트 판교점</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>전북특별자치도 전주시 완산구 팔달로 106-1 한옥마을 주차장 안쪽 1층</t>
+          <t>경기도 성남시 분당구 대왕판교로 660 유스페이스1 1층 125호 챠오바라이트</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>#전주한옥마을한정식맛집, #녹두꽃, #전주녹두꽃, #전주한옥마을한정식, #전주한정식맛집녹두꽃, #전주한옥마을한정식맛집녹두꽃, #전주한정식맛집, #전주한정식, #전주맛집, #전주한옥마을, #전주한옥마을맛집, #한옥마을맛집, #한옥마을한정식맛집, #한옥마을한정식, #전주한상, #전주한상차림, #한정식맛집, #전주, #맛집, #전주건강한맛집</t>
+          <t>#판교맛집, #판교술집, #하이네켄, #하이네켄생맥주, #하이네켄생맥주맛집, #챠오바라이트, #생맥주, #첫모금, #맛집추천, #광고</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2024-08-29 11:30</t>
+          <t>2024-08-29 12:52</t>
         </is>
       </c>
     </row>
@@ -1271,39 +1241,37 @@
           <t>Naver Blog</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>20240828</t>
-        </is>
+      <c r="B21" t="n">
+        <v>20240829</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>홍대 연남동중식당 중화복춘 살롱 시그니처 미쉐린가이드맛집 회식</t>
+          <t>연남동 국숯집 남발카세 팝업 - 젊고 내공 뛰어난 남발게 김준승 셰프님의 새롭고 기발하고 훌륭한 해산물 요리 잔치</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>https://blog.naver.com/rapunzelli3/223564429953</t>
+          <t>https://blog.naver.com/zephyr122059/223559250507</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>중화복춘 살롱 시그니처</t>
+          <t>국숯집 연남점</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>서울특별시 마포구 연남로 10 1층</t>
+          <t>서울특별시 마포구 동교로34길 21 우측 지층</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>#중화복춘, #중화복춘살롱시그니처, #남복춘쉐프, #연남데이트, #연남동중식당, #홍대중식당, #홍대회식, #연남동회식, #홍대미쉐린가이드, #연남동미쉐린가이드, #연남동맛집</t>
+          <t>#남발게님, #국숯집, #연남동국숯집, #남발카세, #해산물잔치, #국숯집팝업, #남발게님팝업, #연남동남발카세팝업</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2024-08-29 11:30</t>
+          <t>2024-08-29 12:52</t>
         </is>
       </c>
     </row>

</xml_diff>